<commit_message>
Update changes to archive initial versions
</commit_message>
<xml_diff>
--- a/Individual/LandmarkSequenceCheck_BaseArch_20250722_b.xlsx
+++ b/Individual/LandmarkSequenceCheck_BaseArch_20250722_b.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\GitHub\PHD_XLS_Validator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\GitHub\PHD_XLS_Validator\Individual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92EDE055-6D90-4B50-94B4-1DE5022657A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EBEDB0-0B17-4FD3-9589-08328EAD8D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21000" activeTab="1" xr2:uid="{B30E8A96-C8BB-4099-9CE9-6C249E4F3EED}"/>
+    <workbookView xWindow="30" yWindow="15" windowWidth="25800" windowHeight="21000" xr2:uid="{B30E8A96-C8BB-4099-9CE9-6C249E4F3EED}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -16312,8 +16312,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S41" sqref="S41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16943,9 +16943,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>